<commit_message>
added thesis and worklog
</commit_message>
<xml_diff>
--- a/Worklog/Worklog Template.xlsx
+++ b/Worklog/Worklog Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phuon\Documents\Research Project\Worklog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BAD77FA-06A0-40A7-90B1-10A6D3FA227A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C538B3FB-A29B-4109-BD91-3B4576DAC233}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D01C876E-0C57-1449-A864-F752FD507052}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="69">
   <si>
     <t>Student Name</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>Start building artefact and doing trail and error</t>
+  </si>
+  <si>
+    <t>Continue building the artefact, testing hyperparameters and fixing errors.</t>
   </si>
 </sst>
 </file>
@@ -647,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC54600-A529-144A-8AA1-058C0E013D1F}">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B35" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62:G66"/>
+    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2183,31 +2186,211 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D67" s="4"/>
+      <c r="A67" t="s">
+        <v>23</v>
+      </c>
+      <c r="B67" t="s">
+        <v>24</v>
+      </c>
+      <c r="C67" t="s">
+        <v>63</v>
+      </c>
+      <c r="D67" s="4">
+        <v>44443</v>
+      </c>
+      <c r="E67">
+        <v>120</v>
+      </c>
+      <c r="F67" t="s">
+        <v>20</v>
+      </c>
+      <c r="G67" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D68" s="4"/>
+      <c r="A68" t="s">
+        <v>23</v>
+      </c>
+      <c r="B68" t="s">
+        <v>24</v>
+      </c>
+      <c r="C68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D68" s="4">
+        <v>44444</v>
+      </c>
+      <c r="E68">
+        <v>120</v>
+      </c>
+      <c r="F68" t="s">
+        <v>20</v>
+      </c>
+      <c r="G68" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D69" s="4"/>
+      <c r="A69" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69" t="s">
+        <v>24</v>
+      </c>
+      <c r="C69" t="s">
+        <v>63</v>
+      </c>
+      <c r="D69" s="4">
+        <v>44445</v>
+      </c>
+      <c r="E69">
+        <v>120</v>
+      </c>
+      <c r="F69" t="s">
+        <v>20</v>
+      </c>
+      <c r="G69" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D70" s="4"/>
+      <c r="A70" t="s">
+        <v>23</v>
+      </c>
+      <c r="B70" t="s">
+        <v>24</v>
+      </c>
+      <c r="C70" t="s">
+        <v>63</v>
+      </c>
+      <c r="D70" s="4">
+        <v>44446</v>
+      </c>
+      <c r="E70">
+        <v>120</v>
+      </c>
+      <c r="F70" t="s">
+        <v>20</v>
+      </c>
+      <c r="G70" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D71" s="4"/>
+      <c r="A71" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71" t="s">
+        <v>24</v>
+      </c>
+      <c r="C71" t="s">
+        <v>63</v>
+      </c>
+      <c r="D71" s="4">
+        <v>44447</v>
+      </c>
+      <c r="E71">
+        <v>120</v>
+      </c>
+      <c r="F71" t="s">
+        <v>20</v>
+      </c>
+      <c r="G71" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D72" s="4"/>
+      <c r="A72" t="s">
+        <v>23</v>
+      </c>
+      <c r="B72" t="s">
+        <v>24</v>
+      </c>
+      <c r="C72" t="s">
+        <v>63</v>
+      </c>
+      <c r="D72" s="4">
+        <v>44448</v>
+      </c>
+      <c r="E72">
+        <v>120</v>
+      </c>
+      <c r="F72" t="s">
+        <v>20</v>
+      </c>
+      <c r="G72" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D73" s="4"/>
+      <c r="A73" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73" t="s">
+        <v>24</v>
+      </c>
+      <c r="C73" t="s">
+        <v>63</v>
+      </c>
+      <c r="D73" s="4">
+        <v>44449</v>
+      </c>
+      <c r="E73">
+        <v>120</v>
+      </c>
+      <c r="F73" t="s">
+        <v>20</v>
+      </c>
+      <c r="G73" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D74" s="4"/>
+      <c r="A74" t="s">
+        <v>23</v>
+      </c>
+      <c r="B74" t="s">
+        <v>24</v>
+      </c>
+      <c r="C74" t="s">
+        <v>63</v>
+      </c>
+      <c r="D74" s="4">
+        <v>44450</v>
+      </c>
+      <c r="E74">
+        <v>120</v>
+      </c>
+      <c r="F74" t="s">
+        <v>20</v>
+      </c>
+      <c r="G74" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D75" s="4"/>
+      <c r="A75" t="s">
+        <v>23</v>
+      </c>
+      <c r="B75" t="s">
+        <v>24</v>
+      </c>
+      <c r="C75" t="s">
+        <v>63</v>
+      </c>
+      <c r="D75" s="4">
+        <v>44451</v>
+      </c>
+      <c r="E75">
+        <v>120</v>
+      </c>
+      <c r="F75" t="s">
+        <v>20</v>
+      </c>
+      <c r="G75" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D76" s="4"/>
@@ -2588,18 +2771,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2621,18 +2804,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99F33CB9-EBB9-4740-8AC2-6F0A2CE058F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33C84895-33C6-4EEF-ADE3-B2C6A0E7CE9B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99F33CB9-EBB9-4740-8AC2-6F0A2CE058F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>